<commit_message>
Elena- boardAdjTargetTest fail except testTargetOccupied().
</commit_message>
<xml_diff>
--- a/data/ClueLayoutTests.xlsx
+++ b/data/ClueLayoutTests.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ecore/Documents/Colorado School of Mines/2021-2022 Junior Year/CSCI 306/Clue/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D07DBA2C-BF5F-2548-A8D2-AECA17B4E09D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B59802DD-1004-5745-B9E3-A427BF0271C7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="460" yWindow="500" windowWidth="16800" windowHeight="20180" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="16020" windowHeight="20180" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -623,7 +623,7 @@
   <dimension ref="A1:X22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="Q24" sqref="Q24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="5.6640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -888,7 +888,7 @@
       <c r="I4" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="J4" s="4" t="s">
+      <c r="J4" s="12" t="s">
         <v>9</v>
       </c>
       <c r="K4" s="1" t="s">
@@ -1098,7 +1098,7 @@
       <c r="G7" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="H7" s="12" t="s">
+      <c r="H7" s="4" t="s">
         <v>9</v>
       </c>
       <c r="I7" s="4" t="s">
@@ -1611,7 +1611,7 @@
       <c r="P14" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="Q14" s="12" t="s">
+      <c r="Q14" s="4" t="s">
         <v>9</v>
       </c>
       <c r="R14" s="4" t="s">
@@ -1656,7 +1656,7 @@
       <c r="H15" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="I15" s="4" t="s">
+      <c r="I15" s="12" t="s">
         <v>9</v>
       </c>
       <c r="J15" s="4" t="s">
@@ -1713,7 +1713,7 @@
       <c r="D16" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="E16" s="12" t="s">
+      <c r="E16" s="4" t="s">
         <v>9</v>
       </c>
       <c r="F16" s="4" t="s">
@@ -1893,7 +1893,7 @@
       <c r="R18" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="S18" s="4" t="s">
+      <c r="S18" s="12" t="s">
         <v>9</v>
       </c>
       <c r="T18" s="6" t="s">

</xml_diff>

<commit_message>
Elena made all boardAdjTest fail. All other tests still either pass/fail.
</commit_message>
<xml_diff>
--- a/data/ClueLayoutTests.xlsx
+++ b/data/ClueLayoutTests.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ecore/Documents/Colorado School of Mines/2021-2022 Junior Year/CSCI 306/Clue/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B59802DD-1004-5745-B9E3-A427BF0271C7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A088B51A-B611-D545-93FE-AC54563E9B1E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="16020" windowHeight="20180" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -157,7 +157,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -165,8 +165,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="13">
+  <fills count="14">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -239,6 +246,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF4B084"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -252,7 +265,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -298,6 +311,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -623,7 +639,7 @@
   <dimension ref="A1:X22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Q24" sqref="Q24"/>
+      <selection activeCell="M17" sqref="M17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="5.6640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -981,7 +997,7 @@
       <c r="P5" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="Q5" s="12" t="s">
+      <c r="Q5" s="17" t="s">
         <v>8</v>
       </c>
       <c r="R5" s="1" t="s">
@@ -1053,7 +1069,7 @@
       <c r="P6" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="Q6" s="4" t="s">
+      <c r="Q6" s="12" t="s">
         <v>9</v>
       </c>
       <c r="R6" s="1" t="s">
@@ -1872,7 +1888,7 @@
       <c r="K18" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="L18" s="7" t="s">
+      <c r="L18" s="12" t="s">
         <v>25</v>
       </c>
       <c r="M18" s="4" t="s">
@@ -1893,7 +1909,7 @@
       <c r="R18" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="S18" s="12" t="s">
+      <c r="S18" s="4" t="s">
         <v>9</v>
       </c>
       <c r="T18" s="6" t="s">

</xml_diff>